<commit_message>
regenerated ES and SHS outputs after merge for CIFMM-2366
</commit_message>
<xml_diff>
--- a/output/EventSummary/patient-dh-base-1.xlsx
+++ b/output/EventSummary/patient-dh-base-1.xlsx
@@ -5557,7 +5557,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>52</v>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F43" t="s" s="2">
         <v>52</v>

</xml_diff>

<commit_message>
Regenerate outputs for ES, SHS and PHR
</commit_message>
<xml_diff>
--- a/output/EventSummary/patient-dh-base-1.xlsx
+++ b/output/EventSummary/patient-dh-base-1.xlsx
@@ -5557,7 +5557,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>52</v>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F43" t="s" s="2">
         <v>52</v>

</xml_diff>

<commit_message>
Generated ES, SHS and PHR outputs.
CIFMM-2340
</commit_message>
<xml_diff>
--- a/output/EventSummary/patient-dh-base-1.xlsx
+++ b/output/EventSummary/patient-dh-base-1.xlsx
@@ -381,10 +381,10 @@
 </t>
   </si>
   <si>
-    <t>Closing the gap registration</t>
-  </si>
-  <si>
-    <t>Closing the Gap registration indicator for an Australian patient.</t>
+    <t>Patient Closing the Gap Program Eligibility Indication</t>
+  </si>
+  <si>
+    <t>Indication for eligibility for the Closing the Gap program.</t>
   </si>
   <si>
     <t>mothersMaidenName</t>
@@ -19860,7 +19860,7 @@
         <v>42</v>
       </c>
       <c r="F155" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G155" t="s" s="2">
         <v>44</v>

</xml_diff>